<commit_message>
organizing and prepping Nisqually data from Craig
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smith.craig\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\24MEW3LM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144C7CF1-CA57-41E8-9B7B-A995025487CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71EFAF6-CE52-4242-965D-6CD44E20B6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="1" activeTab="1" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="1560" yWindow="1230" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="1" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22,6 +22,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -235,10 +244,10 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -260,13 +269,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -274,22 +283,22 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3453,9 +3462,9 @@
       <selection activeCell="L18" sqref="L18:M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>2002</v>
       </c>
@@ -3463,8 +3472,8 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>28</v>
       </c>
       <c r="B2" s="10"/>
@@ -3475,8 +3484,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
       <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -3485,8 +3494,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
       <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -3495,8 +3504,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
       <c r="B5" s="12"/>
       <c r="C5" s="7" t="s">
         <v>0</v>
@@ -3505,8 +3514,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>29</v>
       </c>
       <c r="B6" s="11"/>
@@ -3521,8 +3530,8 @@
         <v>1.6798958464575196E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
       <c r="B7" s="11"/>
       <c r="C7" s="5">
         <v>7.1395573474444579E-4</v>
@@ -3535,8 +3544,8 @@
         <v>3.9952562723266627E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
       <c r="B8" s="11"/>
       <c r="C8" s="5">
         <v>4.6197135777581791E-4</v>
@@ -3549,8 +3558,8 @@
         <v>2.9480731867857399E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
       <c r="B9" s="11"/>
       <c r="C9" s="5">
         <v>0</v>
@@ -3563,8 +3572,8 @@
         <v>2.1273879930221675E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="23">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
         <v>30</v>
       </c>
       <c r="B10" s="10"/>
@@ -3579,8 +3588,8 @@
         <v>2.732582568988496E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
       <c r="B11" s="11"/>
       <c r="C11" s="5">
         <v>4.6197135777581791E-4</v>
@@ -3593,8 +3602,8 @@
         <v>3.1608119860879565E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
       <c r="B12" s="11"/>
       <c r="C12" s="5">
         <v>2.5198437696862794E-4</v>
@@ -3607,8 +3616,8 @@
         <v>1.6853994834475732E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
       <c r="B13" s="12"/>
       <c r="C13" s="7">
         <v>5.0396875393725587E-4</v>
@@ -3621,8 +3630,8 @@
         <v>2.9453213682907131E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
         <v>31</v>
       </c>
       <c r="B14" s="11"/>
@@ -3637,8 +3646,8 @@
         <v>1.5370326876350269E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="11"/>
       <c r="C15" s="5">
         <v>3.1498047121078492E-3</v>
@@ -3651,8 +3660,8 @@
         <v>2.4258575532627915E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
       <c r="B16" s="11"/>
       <c r="C16" s="5">
         <v>1.9318802234261476E-3</v>
@@ -3665,8 +3674,8 @@
         <v>1.4126915902477289E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
       <c r="B17" s="11"/>
       <c r="C17" s="5">
         <v>9.2394271555163582E-4</v>
@@ -3679,8 +3688,8 @@
         <v>9.7254447610113811E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
         <v>32</v>
       </c>
       <c r="B18" s="10">
@@ -3711,8 +3720,8 @@
         <v>1.599295905778612E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
       <c r="B19" s="11">
         <v>4.1233650380884824E-3</v>
       </c>
@@ -3741,8 +3750,8 @@
         <v>1.9048486936224351E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
       <c r="B20" s="11">
         <v>3.2571899616384526E-3</v>
       </c>
@@ -3771,8 +3780,8 @@
         <v>1.1490010928119356E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
       <c r="B21" s="12">
         <v>1.7287727888565248E-3</v>
       </c>
@@ -3801,8 +3810,8 @@
         <v>2.4235604026783007E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
         <v>33</v>
       </c>
       <c r="B22" s="11">
@@ -3833,8 +3842,8 @@
         <v>7.3087499792239677E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
       <c r="B23" s="11">
         <v>1.4194950147529011E-2</v>
       </c>
@@ -3863,8 +3872,8 @@
         <v>0.12397082966702488</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
       <c r="B24" s="11">
         <v>7.3436806318935765E-3</v>
       </c>
@@ -3893,8 +3902,8 @@
         <v>0.15646256387936083</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
       <c r="B25" s="11">
         <v>3.6628544670786935E-3</v>
       </c>
@@ -3923,8 +3932,8 @@
         <v>0.19988009687375935</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="23">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
         <v>34</v>
       </c>
       <c r="B26" s="10">
@@ -3955,8 +3964,8 @@
         <v>0.163898778667595</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
       <c r="B27" s="11">
         <v>2.5266343285465398E-2</v>
       </c>
@@ -3985,8 +3994,8 @@
         <v>0.10791944221741888</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
       <c r="B28" s="11">
         <v>1.2039704459482513E-2</v>
       </c>
@@ -4015,8 +4024,8 @@
         <v>6.5620208687114059E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="22"/>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="23"/>
       <c r="B29" s="12">
         <v>9.2728295861186534E-3</v>
       </c>
@@ -4045,8 +4054,8 @@
         <v>5.0541724872299319E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="23">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
         <v>35</v>
       </c>
       <c r="B30" s="11">
@@ -4077,8 +4086,8 @@
         <v>1.6674139569200188E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
       <c r="B31" s="11">
         <v>2.9542202847108966E-2</v>
       </c>
@@ -4107,8 +4116,8 @@
         <v>2.1423560392975541E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
       <c r="B32" s="11">
         <v>1.7729101706216277E-2</v>
       </c>
@@ -4137,8 +4146,8 @@
         <v>3.8256357844599178E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="22"/>
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="23"/>
       <c r="B33" s="11">
         <v>9.3338145298957759E-3</v>
       </c>
@@ -4167,8 +4176,8 @@
         <v>1.9003660194057031E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="23">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="21">
         <v>36</v>
       </c>
       <c r="B34" s="10">
@@ -4185,8 +4194,8 @@
         <v>3.0718340793254174E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
       <c r="B35" s="11">
         <v>3.3876125778997603E-2</v>
       </c>
@@ -4205,8 +4214,8 @@
         <v>0.55249088507922983</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
       <c r="B36" s="11">
         <v>2.8383823064732316E-2</v>
       </c>
@@ -4221,8 +4230,8 @@
         <v>2.8383823064732316E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23"/>
       <c r="B37" s="12">
         <v>1.7453641994521405E-2</v>
       </c>
@@ -4237,8 +4246,8 @@
         <v>1.7453641994521405E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="23">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
         <v>37</v>
       </c>
       <c r="B38" s="11">
@@ -4255,8 +4264,8 @@
         <v>2.984537104808509E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
       <c r="B39" s="11">
         <v>3.3659534433802346E-2</v>
       </c>
@@ -4271,8 +4280,8 @@
         <v>3.3659534433802346E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
       <c r="B40" s="11">
         <v>2.0552368309434226E-2</v>
       </c>
@@ -4287,8 +4296,8 @@
         <v>2.0552368309434226E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="22"/>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="23"/>
       <c r="B41" s="11">
         <v>6.4953074981427055E-3</v>
       </c>
@@ -4303,8 +4312,8 @@
         <v>6.4953074981427055E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="23">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="21">
         <v>38</v>
       </c>
       <c r="B42" s="10">
@@ -4321,8 +4330,8 @@
         <v>2.3196362872176818E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
       <c r="B43" s="11">
         <v>1.6663926373645208E-2</v>
       </c>
@@ -4337,8 +4346,8 @@
         <v>1.6663926373645208E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
       <c r="B44" s="11">
         <v>1.2766043377454579E-2</v>
       </c>
@@ -4353,8 +4362,8 @@
         <v>1.2766043377454579E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="22"/>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="23"/>
       <c r="B45" s="12">
         <v>6.9981755246819512E-3</v>
       </c>
@@ -4369,8 +4378,8 @@
         <v>6.9981755246819512E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="23">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="21">
         <v>39</v>
       </c>
       <c r="B46" s="11">
@@ -4387,8 +4396,8 @@
         <v>1.225896274565428E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="21"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="22"/>
       <c r="B47" s="11">
         <v>1.0799955727171583E-2</v>
       </c>
@@ -4403,8 +4412,8 @@
         <v>1.0799955727171583E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
       <c r="B48" s="11">
         <v>7.5018690967697038E-3</v>
       </c>
@@ -4419,8 +4428,8 @@
         <v>7.5018690967697038E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="22"/>
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23"/>
       <c r="B49" s="11">
         <v>5.6937796070318488E-3</v>
       </c>
@@ -4435,8 +4444,8 @@
         <v>5.6937796070318488E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="23">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="21">
         <v>40</v>
       </c>
       <c r="B50" s="10">
@@ -4453,8 +4462,8 @@
         <v>8.7128291616953239E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
       <c r="B51" s="11">
         <v>8.9092473543583659E-3</v>
       </c>
@@ -4469,8 +4478,8 @@
         <v>8.9092473543583659E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="22"/>
       <c r="B52" s="11">
         <v>5.7498961550364394E-3</v>
       </c>
@@ -4485,8 +4494,8 @@
         <v>5.7498961550364394E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="22"/>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23"/>
       <c r="B53" s="12">
         <v>4.5518696370374454E-3</v>
       </c>
@@ -4501,8 +4510,8 @@
         <v>4.5518696370374454E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="23">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="21">
         <v>41</v>
       </c>
       <c r="B54" s="11"/>
@@ -4517,8 +4526,8 @@
         <v>3.2323387176646963E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="22"/>
       <c r="B55" s="11"/>
       <c r="C55" s="5">
         <v>2.0578724119104616E-3</v>
@@ -4531,8 +4540,8 @@
         <v>3.2414197186982846E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="21"/>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22"/>
       <c r="B56" s="11"/>
       <c r="C56" s="5">
         <v>7.1395573474444579E-4</v>
@@ -4545,8 +4554,8 @@
         <v>1.7610539427668534E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="22"/>
+    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23"/>
       <c r="B57" s="11"/>
       <c r="C57" s="5">
         <v>1.6798958464575196E-4</v>
@@ -4559,8 +4568,8 @@
         <v>9.7749774939218624E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="23">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
         <v>42</v>
       </c>
       <c r="B58" s="10"/>
@@ -4575,8 +4584,8 @@
         <v>5.7054221222294771E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="21"/>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="22"/>
       <c r="B59" s="11"/>
       <c r="C59" s="5">
         <v>1.2599218848431397E-4</v>
@@ -4589,8 +4598,8 @@
         <v>1.9063937382348702E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="21"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="22"/>
       <c r="B60" s="11"/>
       <c r="C60" s="5">
         <v>3.3597916929150391E-4</v>
@@ -4603,8 +4612,8 @@
         <v>2.9563286422708203E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="22"/>
+    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="23"/>
       <c r="B61" s="12"/>
       <c r="C61" s="7">
         <v>1.2599218848431397E-4</v>
@@ -4617,8 +4626,8 @@
         <v>1.2681773403282201E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="21">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="22">
         <v>43</v>
       </c>
       <c r="B62" s="11"/>
@@ -4633,8 +4642,8 @@
         <v>1.480916139630437E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="21"/>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
       <c r="B63" s="11"/>
       <c r="C63" s="5">
         <v>8.3994792322875979E-5</v>
@@ -4647,8 +4656,8 @@
         <v>6.3271276091659664E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="21"/>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
       <c r="B64" s="11"/>
       <c r="C64" s="5">
         <v>0</v>
@@ -4661,8 +4670,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="22"/>
+    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="23"/>
       <c r="B65" s="11"/>
       <c r="C65" s="5">
         <v>0</v>
@@ -4675,8 +4684,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="23">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="21">
         <v>44</v>
       </c>
       <c r="B66" s="10"/>
@@ -4691,8 +4700,8 @@
         <v>1.0499349040359497E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="21"/>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
       <c r="B67" s="11"/>
       <c r="C67" s="5">
         <v>0</v>
@@ -4705,8 +4714,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="21"/>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="22"/>
       <c r="B68" s="11"/>
       <c r="C68" s="5">
         <v>0</v>
@@ -4719,8 +4728,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="22"/>
+    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="23"/>
       <c r="B69" s="12"/>
       <c r="C69" s="7">
         <v>0</v>
@@ -4733,8 +4742,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="23">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="21">
         <v>45</v>
       </c>
       <c r="B70" s="11"/>
@@ -4749,8 +4758,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="21"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
       <c r="B71" s="11"/>
       <c r="C71" s="5">
         <v>0</v>
@@ -4763,8 +4772,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="21"/>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
       <c r="B72" s="11"/>
       <c r="C72" s="5">
         <v>0</v>
@@ -4777,8 +4786,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="22"/>
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="23"/>
       <c r="B73" s="11"/>
       <c r="C73" s="5">
         <v>0</v>
@@ -4791,8 +4800,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="23">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="21">
         <v>46</v>
       </c>
       <c r="B74" s="10"/>
@@ -4807,8 +4816,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="21"/>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
       <c r="B75" s="11"/>
       <c r="C75" s="5">
         <v>0</v>
@@ -4821,8 +4830,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="21"/>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
       <c r="B76" s="11"/>
       <c r="C76" s="5">
         <v>0</v>
@@ -4835,8 +4844,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="22"/>
+    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="23"/>
       <c r="B77" s="12"/>
       <c r="C77" s="7">
         <v>0</v>
@@ -4851,6 +4860,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A66:A69"/>
     <mergeCell ref="A70:A73"/>
     <mergeCell ref="A74:A77"/>
     <mergeCell ref="A2:A5"/>
@@ -4867,9 +4879,6 @@
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A62:A65"/>
     <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A66:A69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4881,12 +4890,12 @@
   <dimension ref="D4:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L4" t="s">
         <v>1</v>
       </c>
@@ -4897,7 +4906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L5">
         <v>29</v>
       </c>
@@ -4908,7 +4917,7 @@
         <v>1.599295905778612E-3</v>
       </c>
     </row>
-    <row r="6" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L6">
         <v>30</v>
       </c>
@@ -4919,7 +4928,7 @@
         <v>1.9048486936224351E-3</v>
       </c>
     </row>
-    <row r="7" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L7">
         <v>31</v>
       </c>
@@ -4933,7 +4942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L8">
         <v>32</v>
       </c>
@@ -4944,7 +4953,7 @@
         <v>2.4235604026783007E-2</v>
       </c>
     </row>
-    <row r="9" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L9">
         <v>33</v>
       </c>
@@ -4955,7 +4964,7 @@
         <v>7.3087499792239677E-2</v>
       </c>
     </row>
-    <row r="10" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L10">
         <v>34</v>
       </c>
@@ -4966,7 +4975,7 @@
         <v>0.12397082966702488</v>
       </c>
     </row>
-    <row r="11" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L11">
         <v>35</v>
       </c>
@@ -4977,7 +4986,7 @@
         <v>0.15646256387936083</v>
       </c>
     </row>
-    <row r="12" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L12">
         <v>36</v>
       </c>
@@ -4988,7 +4997,7 @@
         <v>0.19988009687375935</v>
       </c>
     </row>
-    <row r="13" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L13">
         <v>37</v>
       </c>
@@ -4999,7 +5008,7 @@
         <v>0.163898778667595</v>
       </c>
     </row>
-    <row r="14" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L14">
         <v>38</v>
       </c>
@@ -5010,7 +5019,7 @@
         <v>0.10791944221741888</v>
       </c>
     </row>
-    <row r="15" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L15">
         <v>39</v>
       </c>
@@ -5021,7 +5030,7 @@
         <v>6.5620208687114059E-2</v>
       </c>
     </row>
-    <row r="16" spans="12:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L16">
         <v>40</v>
       </c>
@@ -5032,7 +5041,7 @@
         <v>5.0541724872299319E-2</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="L17">
         <v>41</v>
       </c>
@@ -5043,7 +5052,7 @@
         <v>1.6674139569200188E-2</v>
       </c>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="L18">
         <v>42</v>
       </c>
@@ -5054,7 +5063,7 @@
         <v>2.1423560392975541E-3</v>
       </c>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="L19">
         <v>43</v>
       </c>
@@ -5065,7 +5074,7 @@
         <v>3.8256357844599178E-4</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="L20">
         <v>44</v>
       </c>
@@ -5076,12 +5085,12 @@
         <v>1.9003660194057031E-4</v>
       </c>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -5100,14 +5109,14 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>32</v>
       </c>
@@ -5118,7 +5127,7 @@
         <v>3.8461538461538464E-2</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>33</v>
       </c>
@@ -5129,7 +5138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>34</v>
       </c>
@@ -5140,7 +5149,7 @@
         <v>3.8461538461538464E-2</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>35</v>
       </c>
@@ -5151,7 +5160,7 @@
         <v>5.128205128205128E-2</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>36</v>
       </c>
@@ -5162,7 +5171,7 @@
         <v>3.8461538461538464E-2</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>37</v>
       </c>
@@ -5173,7 +5182,7 @@
         <v>8.9743589743589744E-2</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>38</v>
       </c>
@@ -5184,7 +5193,7 @@
         <v>0.14102564102564102</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>39</v>
       </c>
@@ -5195,7 +5204,7 @@
         <v>6.4102564102564097E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>40</v>
       </c>
@@ -5206,7 +5215,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>41</v>
       </c>
@@ -5217,7 +5226,7 @@
         <v>5.128205128205128E-2</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>42</v>
       </c>
@@ -5228,7 +5237,7 @@
         <v>8.9743589743589744E-2</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>43</v>
       </c>
@@ -5239,7 +5248,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>44</v>
       </c>
@@ -5250,7 +5259,7 @@
         <v>0.14102564102564102</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>45</v>
       </c>
@@ -5261,7 +5270,7 @@
         <v>8.9743589743589744E-2</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>46</v>
       </c>
@@ -5272,17 +5281,17 @@
         <v>1.282051282051282E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -5301,9 +5310,9 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
@@ -5314,7 +5323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="18">
         <v>47</v>
       </c>
@@ -5325,7 +5334,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
         <v>48</v>
       </c>
@@ -5336,7 +5345,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <v>49</v>
       </c>
@@ -5347,7 +5356,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="18">
         <v>50</v>
       </c>
@@ -5358,7 +5367,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="18">
         <v>51</v>
       </c>
@@ -5369,7 +5378,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="18">
         <v>52</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="18">
         <v>53</v>
       </c>
@@ -5391,7 +5400,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="18">
         <v>54</v>
       </c>
@@ -5402,7 +5411,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="18">
         <v>55</v>
       </c>
@@ -5413,7 +5422,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="18">
         <v>56</v>
       </c>
@@ -5424,22 +5433,22 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>14</v>
       </c>
@@ -5451,11 +5460,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5659,26 +5669,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5702,9 +5703,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
data is caught up I think!
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71EFAF6-CE52-4242-965D-6CD44E20B6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D24D27D-7200-420F-A145-8BD8DDA7D07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1230" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="1" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-28185" yWindow="5985" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -4889,7 +4889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5AB5EB-5F17-4CB3-ADB0-B51E1B4ACDBA}">
   <dimension ref="D4:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -5105,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6174EEDB-7B7A-44D2-9EE9-2214797252C5}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5307,7 +5307,7 @@
   <dimension ref="B3:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adjusted some timing for locnis
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D24D27D-7200-420F-A145-8BD8DDA7D07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021E1C00-2692-477C-BFC1-D0DC4F1BEDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28185" yWindow="5985" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="2370" yWindow="630" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t/>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Runsize range 2k-62k. Average 27k</t>
+  </si>
+  <si>
+    <t>Gauntlet</t>
+  </si>
+  <si>
+    <t>RM 13</t>
   </si>
 </sst>
 </file>
@@ -133,12 +139,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -242,7 +254,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,6 +313,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1128,7 +1144,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'LocNis Chinook'!$C$2:$C$16</c:f>
+              <c:f>'LocNis Chinook'!$C$6:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1182,7 +1198,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'LocNis Chinook'!$E$2:$E$16</c:f>
+              <c:f>'LocNis Chinook'!$E$6:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3124,13 +3140,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4860,25 +4876,25 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="A66:A69"/>
     <mergeCell ref="A70:A73"/>
     <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A38:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5103,196 +5119,290 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6174EEDB-7B7A-44D2-9EE9-2214797252C5}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C2" sqref="C2:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="24">
+        <v>29</v>
+      </c>
+      <c r="D3" s="26">
+        <v>45489</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="24">
+        <v>30</v>
+      </c>
+      <c r="D4" s="26">
+        <v>45496</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="24">
+        <v>31</v>
+      </c>
+      <c r="D5" s="26">
+        <v>45503</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="27">
+        <v>3.8461538461538464E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
         <v>32</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D6" s="17">
         <v>45510</v>
-      </c>
-      <c r="E2" s="15">
-        <v>3.8461538461538464E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>33</v>
-      </c>
-      <c r="D3" s="17">
-        <v>45517</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>34</v>
-      </c>
-      <c r="D4" s="17">
-        <v>45524</v>
-      </c>
-      <c r="E4" s="15">
-        <v>3.8461538461538464E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>35</v>
-      </c>
-      <c r="D5" s="17">
-        <v>45531</v>
-      </c>
-      <c r="E5" s="15">
-        <v>5.128205128205128E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>36</v>
-      </c>
-      <c r="D6" s="17">
-        <v>45538</v>
       </c>
       <c r="E6" s="15">
         <v>3.8461538461538464E-2</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7" s="17">
+        <v>45517</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
+        <v>3.8461538461538464E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>34</v>
+      </c>
+      <c r="D8" s="17">
+        <v>45524</v>
+      </c>
+      <c r="E8" s="15">
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F8" s="27">
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>35</v>
+      </c>
+      <c r="D9" s="17">
+        <v>45531</v>
+      </c>
+      <c r="E9" s="15">
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="F9" s="27">
+        <v>3.8461538461538464E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10" s="17">
+        <v>45538</v>
+      </c>
+      <c r="E10" s="15">
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F10" s="27">
+        <v>8.9743589743589744E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11">
         <v>37</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D11" s="17">
         <v>45545</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E11" s="15">
         <v>8.9743589743589744E-2</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8">
+      <c r="F11" s="27">
+        <v>0.14102564102564102</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>38</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D12" s="17">
         <v>45552</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E12" s="15">
         <v>0.14102564102564102</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9">
+      <c r="F12" s="27">
+        <v>6.4102564102564097E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13">
         <v>39</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D13" s="17">
         <v>45559</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E13" s="15">
         <v>6.4102564102564097E-2</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10">
+      <c r="F13" s="27">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14">
         <v>40</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D14" s="17">
         <v>45566</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E14" s="15">
         <v>7.6923076923076927E-2</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11">
+      <c r="F14" s="27">
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15">
         <v>41</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D15" s="17">
         <v>45573</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E15" s="15">
         <v>5.128205128205128E-2</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12">
+      <c r="F15" s="27">
+        <v>8.9743589743589744E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16">
         <v>42</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D16" s="17">
         <v>45580</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E16" s="15">
         <v>8.9743589743589744E-2</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13">
+      <c r="F16" s="27">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17">
         <v>43</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D17" s="17">
         <v>45587</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E17" s="15">
         <v>7.6923076923076927E-2</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14">
+      <c r="F17" s="27">
+        <v>0.14102564102564102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18">
         <v>44</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D18" s="17">
         <v>45594</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E18" s="15">
         <v>0.14102564102564102</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15">
+      <c r="F18" s="27">
+        <v>8.9743589743589744E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19">
         <v>45</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D19" s="17">
         <v>45601</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E19" s="15">
         <v>8.9743589743589744E-2</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16">
+      <c r="F19" s="27">
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20">
         <v>46</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D20" s="17">
         <v>45608</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E20" s="15">
         <v>1.282051282051282E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="F20" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5460,12 +5570,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5669,17 +5778,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5703,17 +5821,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
end of day saves
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F9D06C-5AD8-49C0-88E6-FECB00DAB72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AC23DF-760E-4C96-82BC-FAE77EFC01B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="5985" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-28395" yWindow="7950" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>

</xml_diff>

<commit_message>
updated with some initial thoughts about pinnipeds
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AC23DF-760E-4C96-82BC-FAE77EFC01B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365F9DEE-FF8E-46B7-8F10-9B9EF2D5DB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28395" yWindow="7950" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-27990" yWindow="5715" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -263,7 +263,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,6 +313,10 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -322,10 +326,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3498,7 +3499,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="25">
         <v>28</v>
       </c>
       <c r="B2" s="10"/>
@@ -3510,7 +3511,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -3520,7 +3521,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -3530,7 +3531,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="12"/>
       <c r="C5" s="7" t="s">
         <v>0</v>
@@ -3540,7 +3541,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="25">
         <v>29</v>
       </c>
       <c r="B6" s="11"/>
@@ -3556,7 +3557,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="11"/>
       <c r="C7" s="5">
         <v>7.1395573474444579E-4</v>
@@ -3570,7 +3571,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="11"/>
       <c r="C8" s="5">
         <v>4.6197135777581791E-4</v>
@@ -3584,7 +3585,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="11"/>
       <c r="C9" s="5">
         <v>0</v>
@@ -3598,7 +3599,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="25">
         <v>30</v>
       </c>
       <c r="B10" s="10"/>
@@ -3614,7 +3615,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="11"/>
       <c r="C11" s="5">
         <v>4.6197135777581791E-4</v>
@@ -3628,7 +3629,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="11"/>
       <c r="C12" s="5">
         <v>2.5198437696862794E-4</v>
@@ -3642,7 +3643,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="12"/>
       <c r="C13" s="7">
         <v>5.0396875393725587E-4</v>
@@ -3656,7 +3657,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="25">
         <v>31</v>
       </c>
       <c r="B14" s="11"/>
@@ -3672,7 +3673,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="11"/>
       <c r="C15" s="5">
         <v>3.1498047121078492E-3</v>
@@ -3686,7 +3687,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="11"/>
       <c r="C16" s="5">
         <v>1.9318802234261476E-3</v>
@@ -3700,7 +3701,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="11"/>
       <c r="C17" s="5">
         <v>9.2394271555163582E-4</v>
@@ -3714,7 +3715,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="25">
         <v>32</v>
       </c>
       <c r="B18" s="10">
@@ -3746,7 +3747,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="11">
         <v>4.1233650380884824E-3</v>
       </c>
@@ -3776,7 +3777,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="11">
         <v>3.2571899616384526E-3</v>
       </c>
@@ -3806,7 +3807,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="12">
         <v>1.7287727888565248E-3</v>
       </c>
@@ -3836,7 +3837,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="25">
         <v>33</v>
       </c>
       <c r="B22" s="11">
@@ -3868,7 +3869,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="11">
         <v>1.4194950147529011E-2</v>
       </c>
@@ -3898,7 +3899,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="11">
         <v>7.3436806318935765E-3</v>
       </c>
@@ -3928,7 +3929,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="11">
         <v>3.6628544670786935E-3</v>
       </c>
@@ -3958,7 +3959,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
+      <c r="A26" s="25">
         <v>34</v>
       </c>
       <c r="B26" s="10">
@@ -3990,7 +3991,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="11">
         <v>2.5266343285465398E-2</v>
       </c>
@@ -4020,7 +4021,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="11">
         <v>1.2039704459482513E-2</v>
       </c>
@@ -4050,7 +4051,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="12">
         <v>9.2728295861186534E-3</v>
       </c>
@@ -4080,7 +4081,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="21">
+      <c r="A30" s="25">
         <v>35</v>
       </c>
       <c r="B30" s="11">
@@ -4112,7 +4113,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="11">
         <v>2.9542202847108966E-2</v>
       </c>
@@ -4142,7 +4143,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="11">
         <v>1.7729101706216277E-2</v>
       </c>
@@ -4172,7 +4173,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="11">
         <v>9.3338145298957759E-3</v>
       </c>
@@ -4202,7 +4203,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="21">
+      <c r="A34" s="25">
         <v>36</v>
       </c>
       <c r="B34" s="10">
@@ -4220,7 +4221,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="11">
         <v>3.3876125778997603E-2</v>
       </c>
@@ -4240,7 +4241,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="11">
         <v>2.8383823064732316E-2</v>
       </c>
@@ -4256,7 +4257,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="12">
         <v>1.7453641994521405E-2</v>
       </c>
@@ -4272,7 +4273,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="21">
+      <c r="A38" s="25">
         <v>37</v>
       </c>
       <c r="B38" s="11">
@@ -4290,7 +4291,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="11">
         <v>3.3659534433802346E-2</v>
       </c>
@@ -4306,7 +4307,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="11">
         <v>2.0552368309434226E-2</v>
       </c>
@@ -4322,7 +4323,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="11">
         <v>6.4953074981427055E-3</v>
       </c>
@@ -4338,7 +4339,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="21">
+      <c r="A42" s="25">
         <v>38</v>
       </c>
       <c r="B42" s="10">
@@ -4356,7 +4357,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="11">
         <v>1.6663926373645208E-2</v>
       </c>
@@ -4372,7 +4373,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="11">
         <v>1.2766043377454579E-2</v>
       </c>
@@ -4388,7 +4389,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="12">
         <v>6.9981755246819512E-3</v>
       </c>
@@ -4404,7 +4405,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="21">
+      <c r="A46" s="25">
         <v>39</v>
       </c>
       <c r="B46" s="11">
@@ -4422,7 +4423,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="11">
         <v>1.0799955727171583E-2</v>
       </c>
@@ -4438,7 +4439,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="11">
         <v>7.5018690967697038E-3</v>
       </c>
@@ -4454,7 +4455,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="11">
         <v>5.6937796070318488E-3</v>
       </c>
@@ -4470,7 +4471,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="21">
+      <c r="A50" s="25">
         <v>40</v>
       </c>
       <c r="B50" s="10">
@@ -4488,7 +4489,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="11">
         <v>8.9092473543583659E-3</v>
       </c>
@@ -4504,7 +4505,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="11">
         <v>5.7498961550364394E-3</v>
       </c>
@@ -4520,7 +4521,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="23"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="12">
         <v>4.5518696370374454E-3</v>
       </c>
@@ -4536,7 +4537,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="21">
+      <c r="A54" s="25">
         <v>41</v>
       </c>
       <c r="B54" s="11"/>
@@ -4552,7 +4553,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="11"/>
       <c r="C55" s="5">
         <v>2.0578724119104616E-3</v>
@@ -4566,7 +4567,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="11"/>
       <c r="C56" s="5">
         <v>7.1395573474444579E-4</v>
@@ -4580,7 +4581,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="23"/>
+      <c r="A57" s="27"/>
       <c r="B57" s="11"/>
       <c r="C57" s="5">
         <v>1.6798958464575196E-4</v>
@@ -4594,7 +4595,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="21">
+      <c r="A58" s="25">
         <v>42</v>
       </c>
       <c r="B58" s="10"/>
@@ -4610,7 +4611,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="11"/>
       <c r="C59" s="5">
         <v>1.2599218848431397E-4</v>
@@ -4624,7 +4625,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="11"/>
       <c r="C60" s="5">
         <v>3.3597916929150391E-4</v>
@@ -4638,7 +4639,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="23"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="12"/>
       <c r="C61" s="7">
         <v>1.2599218848431397E-4</v>
@@ -4652,7 +4653,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
+      <c r="A62" s="26">
         <v>43</v>
       </c>
       <c r="B62" s="11"/>
@@ -4668,7 +4669,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="11"/>
       <c r="C63" s="5">
         <v>8.3994792322875979E-5</v>
@@ -4682,7 +4683,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="11"/>
       <c r="C64" s="5">
         <v>0</v>
@@ -4696,7 +4697,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="23"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="11"/>
       <c r="C65" s="5">
         <v>0</v>
@@ -4710,7 +4711,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="21">
+      <c r="A66" s="25">
         <v>44</v>
       </c>
       <c r="B66" s="10"/>
@@ -4726,7 +4727,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="11"/>
       <c r="C67" s="5">
         <v>0</v>
@@ -4740,7 +4741,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="11"/>
       <c r="C68" s="5">
         <v>0</v>
@@ -4754,7 +4755,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="23"/>
+      <c r="A69" s="27"/>
       <c r="B69" s="12"/>
       <c r="C69" s="7">
         <v>0</v>
@@ -4768,7 +4769,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="21">
+      <c r="A70" s="25">
         <v>45</v>
       </c>
       <c r="B70" s="11"/>
@@ -4784,7 +4785,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="11"/>
       <c r="C71" s="5">
         <v>0</v>
@@ -4798,7 +4799,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="11"/>
       <c r="C72" s="5">
         <v>0</v>
@@ -4812,7 +4813,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="23"/>
+      <c r="A73" s="27"/>
       <c r="B73" s="11"/>
       <c r="C73" s="5">
         <v>0</v>
@@ -4826,7 +4827,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="21">
+      <c r="A74" s="25">
         <v>46</v>
       </c>
       <c r="B74" s="10"/>
@@ -4842,7 +4843,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="22"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="11"/>
       <c r="C75" s="5">
         <v>0</v>
@@ -4856,7 +4857,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="11"/>
       <c r="C76" s="5">
         <v>0</v>
@@ -4870,7 +4871,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="23"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="12"/>
       <c r="C77" s="7">
         <v>0</v>
@@ -4885,25 +4886,25 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4944,7 +4945,7 @@
       <c r="N5" s="16">
         <v>1.599295905778612E-3</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="21">
         <f>N5*22000</f>
         <v>35.184509927129461</v>
       </c>
@@ -4959,7 +4960,7 @@
       <c r="N6" s="16">
         <v>1.9048486936224351E-3</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="21">
         <f t="shared" ref="O6:O20" si="0">N6*22000</f>
         <v>41.906671259693574</v>
       </c>
@@ -4974,7 +4975,7 @@
       <c r="N7" s="16">
         <v>1.1490010928119356E-2</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="21">
         <f t="shared" si="0"/>
         <v>252.78024041862582</v>
       </c>
@@ -4992,7 +4993,7 @@
       <c r="N8" s="16">
         <v>2.4235604026783007E-2</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="21">
         <f t="shared" si="0"/>
         <v>533.18328858922621</v>
       </c>
@@ -5007,7 +5008,7 @@
       <c r="N9" s="16">
         <v>7.3087499792239677E-2</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="21">
         <f t="shared" si="0"/>
         <v>1607.9249954292729</v>
       </c>
@@ -5022,7 +5023,7 @@
       <c r="N10" s="16">
         <v>0.12397082966702488</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10" s="21">
         <f t="shared" si="0"/>
         <v>2727.3582526745477</v>
       </c>
@@ -5037,7 +5038,7 @@
       <c r="N11" s="16">
         <v>0.15646256387936083</v>
       </c>
-      <c r="O11" s="24">
+      <c r="O11" s="21">
         <f t="shared" si="0"/>
         <v>3442.1764053459383</v>
       </c>
@@ -5052,7 +5053,7 @@
       <c r="N12" s="16">
         <v>0.19988009687375935</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="21">
         <f t="shared" si="0"/>
         <v>4397.362131222706</v>
       </c>
@@ -5067,7 +5068,7 @@
       <c r="N13" s="16">
         <v>0.163898778667595</v>
       </c>
-      <c r="O13" s="24">
+      <c r="O13" s="21">
         <f t="shared" si="0"/>
         <v>3605.7731306870901</v>
       </c>
@@ -5082,7 +5083,7 @@
       <c r="N14" s="16">
         <v>0.10791944221741888</v>
       </c>
-      <c r="O14" s="24">
+      <c r="O14" s="21">
         <f t="shared" si="0"/>
         <v>2374.2277287832153</v>
       </c>
@@ -5097,7 +5098,7 @@
       <c r="N15" s="16">
         <v>6.5620208687114059E-2</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15" s="21">
         <f t="shared" si="0"/>
         <v>1443.6445911165092</v>
       </c>
@@ -5112,7 +5113,7 @@
       <c r="N16" s="16">
         <v>5.0541724872299319E-2</v>
       </c>
-      <c r="O16" s="24">
+      <c r="O16" s="21">
         <f t="shared" si="0"/>
         <v>1111.917947190585</v>
       </c>
@@ -5127,7 +5128,7 @@
       <c r="N17" s="16">
         <v>1.6674139569200188E-2</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17" s="21">
         <f t="shared" si="0"/>
         <v>366.83107052240416</v>
       </c>
@@ -5142,7 +5143,7 @@
       <c r="N18" s="16">
         <v>2.1423560392975541E-3</v>
       </c>
-      <c r="O18" s="24">
+      <c r="O18" s="21">
         <f t="shared" si="0"/>
         <v>47.13183286454619</v>
       </c>
@@ -5157,7 +5158,7 @@
       <c r="N19" s="16">
         <v>3.8256357844599178E-4</v>
       </c>
-      <c r="O19" s="24">
+      <c r="O19" s="21">
         <f t="shared" si="0"/>
         <v>8.4163987258118187</v>
       </c>
@@ -5172,7 +5173,7 @@
       <c r="N20" s="16">
         <v>1.9003660194057031E-4</v>
       </c>
-      <c r="O20" s="24">
+      <c r="O20" s="21">
         <f t="shared" si="0"/>
         <v>4.1808052426925473</v>
       </c>
@@ -5198,7 +5199,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5221,53 +5222,53 @@
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="24">
+      <c r="C3" s="21">
         <v>29</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="23">
         <v>45489</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25">
+      <c r="E3" s="21"/>
+      <c r="F3" s="22">
         <v>0.01</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="21">
         <f>630 * F3</f>
         <v>6.3</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="24">
+      <c r="C4" s="21">
         <v>30</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="23">
         <v>45496</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <v>0.01</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="22">
         <v>0.01</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="21">
         <f t="shared" ref="G4:G20" si="0">630 * F4</f>
         <v>6.3</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="24">
+      <c r="C5" s="21">
         <v>31</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="23">
         <v>45503</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
         <v>0.01</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="24">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>24.230769230769234</v>
       </c>
@@ -5282,10 +5283,10 @@
       <c r="E6" s="15">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="24">
         <v>0</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5300,10 +5301,10 @@
       <c r="E7" s="15">
         <v>0</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="24">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="21">
         <f t="shared" si="0"/>
         <v>24.230769230769234</v>
       </c>
@@ -5318,10 +5319,10 @@
       <c r="E8" s="15">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="24">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="21">
         <f t="shared" si="0"/>
         <v>32.307692307692307</v>
       </c>
@@ -5336,10 +5337,10 @@
       <c r="E9" s="15">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="24">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="21">
         <f t="shared" si="0"/>
         <v>24.230769230769234</v>
       </c>
@@ -5354,10 +5355,10 @@
       <c r="E10" s="15">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="24">
         <v>8.9743589743589744E-2</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <f t="shared" si="0"/>
         <v>56.53846153846154</v>
       </c>
@@ -5372,10 +5373,10 @@
       <c r="E11" s="15">
         <v>8.9743589743589744E-2</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="24">
         <v>0.14102564102564102</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="21">
         <f t="shared" si="0"/>
         <v>88.84615384615384</v>
       </c>
@@ -5390,10 +5391,10 @@
       <c r="E12" s="15">
         <v>0.14102564102564102</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="24">
         <v>6.4102564102564097E-2</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="21">
         <f t="shared" si="0"/>
         <v>40.38461538461538</v>
       </c>
@@ -5408,10 +5409,10 @@
       <c r="E13" s="15">
         <v>6.4102564102564097E-2</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="24">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="21">
         <f t="shared" si="0"/>
         <v>48.461538461538467</v>
       </c>
@@ -5426,10 +5427,10 @@
       <c r="E14" s="15">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="24">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="21">
         <f t="shared" si="0"/>
         <v>32.307692307692307</v>
       </c>
@@ -5444,10 +5445,10 @@
       <c r="E15" s="15">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="24">
         <v>8.9743589743589744E-2</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="21">
         <f t="shared" si="0"/>
         <v>56.53846153846154</v>
       </c>
@@ -5462,10 +5463,10 @@
       <c r="E16" s="15">
         <v>8.9743589743589744E-2</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="24">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <f t="shared" si="0"/>
         <v>48.461538461538467</v>
       </c>
@@ -5480,10 +5481,10 @@
       <c r="E17" s="15">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="24">
         <v>0.14102564102564102</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="21">
         <f t="shared" si="0"/>
         <v>88.84615384615384</v>
       </c>
@@ -5498,10 +5499,10 @@
       <c r="E18" s="15">
         <v>0.14102564102564102</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="24">
         <v>8.9743589743589744E-2</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="21">
         <f t="shared" si="0"/>
         <v>56.53846153846154</v>
       </c>
@@ -5516,10 +5517,10 @@
       <c r="E19" s="15">
         <v>8.9743589743589744E-2</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="24">
         <v>1.282051282051282E-2</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="21">
         <f t="shared" si="0"/>
         <v>8.0769230769230766</v>
       </c>
@@ -5534,12 +5535,22 @@
       <c r="E20" s="15">
         <v>1.282051282051282E-2</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="22">
         <v>0</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="28">
+        <f>SUM(F3:F20)</f>
+        <v>1.0199999999999998</v>
+      </c>
+      <c r="G21" s="21">
+        <f>SUM(G3:G20)</f>
+        <v>642.6</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5568,7 +5579,7 @@
   <dimension ref="B3:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5597,7 +5608,7 @@
       <c r="D4" s="20">
         <v>0.02</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="21">
         <f>D4*27000</f>
         <v>540</v>
       </c>
@@ -5612,7 +5623,7 @@
       <c r="D5" s="20">
         <v>0.04</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="21">
         <f t="shared" ref="E5:E13" si="0">D5*27000</f>
         <v>1080</v>
       </c>
@@ -5627,7 +5638,7 @@
       <c r="D6" s="20">
         <v>0.1</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <f t="shared" si="0"/>
         <v>2700</v>
       </c>
@@ -5642,7 +5653,7 @@
       <c r="D7" s="20">
         <v>0.17</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="21">
         <f t="shared" si="0"/>
         <v>4590</v>
       </c>
@@ -5657,7 +5668,7 @@
       <c r="D8" s="20">
         <v>0.21</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <f t="shared" si="0"/>
         <v>5670</v>
       </c>
@@ -5672,7 +5683,7 @@
       <c r="D9" s="20">
         <v>0.19</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <f t="shared" si="0"/>
         <v>5130</v>
       </c>
@@ -5687,7 +5698,7 @@
       <c r="D10" s="20">
         <v>0.15</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <f t="shared" si="0"/>
         <v>4050</v>
       </c>
@@ -5702,7 +5713,7 @@
       <c r="D11" s="20">
         <v>0.09</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <f t="shared" si="0"/>
         <v>2430</v>
       </c>
@@ -5717,7 +5728,7 @@
       <c r="D12" s="20">
         <v>0.02</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="21">
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
@@ -5732,9 +5743,15 @@
       <c r="D13" s="20">
         <v>0.01</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="21">
         <f t="shared" si="0"/>
         <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="28">
+        <f>SUM(D4:D13)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -5764,11 +5781,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5972,26 +5990,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6015,9 +6024,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
checking for fishing season info
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365F9DEE-FF8E-46B7-8F10-9B9EF2D5DB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1758102-C42F-4C1A-9D36-173235FAB1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="5715" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-27990" yWindow="5715" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="3" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -317,6 +317,7 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -326,7 +327,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3499,7 +3499,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+      <c r="A2" s="26">
         <v>28</v>
       </c>
       <c r="B2" s="10"/>
@@ -3511,7 +3511,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -3521,7 +3521,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -3531,7 +3531,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="12"/>
       <c r="C5" s="7" t="s">
         <v>0</v>
@@ -3541,7 +3541,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="26">
         <v>29</v>
       </c>
       <c r="B6" s="11"/>
@@ -3557,7 +3557,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="11"/>
       <c r="C7" s="5">
         <v>7.1395573474444579E-4</v>
@@ -3571,7 +3571,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="11"/>
       <c r="C8" s="5">
         <v>4.6197135777581791E-4</v>
@@ -3585,7 +3585,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="11"/>
       <c r="C9" s="5">
         <v>0</v>
@@ -3599,7 +3599,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="26">
         <v>30</v>
       </c>
       <c r="B10" s="10"/>
@@ -3615,7 +3615,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="11"/>
       <c r="C11" s="5">
         <v>4.6197135777581791E-4</v>
@@ -3629,7 +3629,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="11"/>
       <c r="C12" s="5">
         <v>2.5198437696862794E-4</v>
@@ -3643,7 +3643,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="12"/>
       <c r="C13" s="7">
         <v>5.0396875393725587E-4</v>
@@ -3657,7 +3657,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
+      <c r="A14" s="26">
         <v>31</v>
       </c>
       <c r="B14" s="11"/>
@@ -3673,7 +3673,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="11"/>
       <c r="C15" s="5">
         <v>3.1498047121078492E-3</v>
@@ -3687,7 +3687,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="11"/>
       <c r="C16" s="5">
         <v>1.9318802234261476E-3</v>
@@ -3701,7 +3701,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="11"/>
       <c r="C17" s="5">
         <v>9.2394271555163582E-4</v>
@@ -3715,7 +3715,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="A18" s="26">
         <v>32</v>
       </c>
       <c r="B18" s="10">
@@ -3747,7 +3747,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="11">
         <v>4.1233650380884824E-3</v>
       </c>
@@ -3777,7 +3777,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="11">
         <v>3.2571899616384526E-3</v>
       </c>
@@ -3807,7 +3807,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="12">
         <v>1.7287727888565248E-3</v>
       </c>
@@ -3837,7 +3837,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
+      <c r="A22" s="26">
         <v>33</v>
       </c>
       <c r="B22" s="11">
@@ -3869,7 +3869,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="11">
         <v>1.4194950147529011E-2</v>
       </c>
@@ -3899,7 +3899,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="11">
         <v>7.3436806318935765E-3</v>
       </c>
@@ -3929,7 +3929,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="11">
         <v>3.6628544670786935E-3</v>
       </c>
@@ -3959,7 +3959,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="25">
+      <c r="A26" s="26">
         <v>34</v>
       </c>
       <c r="B26" s="10">
@@ -3991,7 +3991,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="11">
         <v>2.5266343285465398E-2</v>
       </c>
@@ -4021,7 +4021,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="11">
         <v>1.2039704459482513E-2</v>
       </c>
@@ -4051,7 +4051,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="12">
         <v>9.2728295861186534E-3</v>
       </c>
@@ -4081,7 +4081,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="25">
+      <c r="A30" s="26">
         <v>35</v>
       </c>
       <c r="B30" s="11">
@@ -4113,7 +4113,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="11">
         <v>2.9542202847108966E-2</v>
       </c>
@@ -4143,7 +4143,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="11">
         <v>1.7729101706216277E-2</v>
       </c>
@@ -4173,7 +4173,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="11">
         <v>9.3338145298957759E-3</v>
       </c>
@@ -4203,7 +4203,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="25">
+      <c r="A34" s="26">
         <v>36</v>
       </c>
       <c r="B34" s="10">
@@ -4221,7 +4221,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="11">
         <v>3.3876125778997603E-2</v>
       </c>
@@ -4241,7 +4241,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="11">
         <v>2.8383823064732316E-2</v>
       </c>
@@ -4257,7 +4257,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="12">
         <v>1.7453641994521405E-2</v>
       </c>
@@ -4273,7 +4273,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="25">
+      <c r="A38" s="26">
         <v>37</v>
       </c>
       <c r="B38" s="11">
@@ -4291,7 +4291,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="11">
         <v>3.3659534433802346E-2</v>
       </c>
@@ -4307,7 +4307,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="11">
         <v>2.0552368309434226E-2</v>
       </c>
@@ -4323,7 +4323,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="11">
         <v>6.4953074981427055E-3</v>
       </c>
@@ -4339,7 +4339,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="25">
+      <c r="A42" s="26">
         <v>38</v>
       </c>
       <c r="B42" s="10">
@@ -4357,7 +4357,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="11">
         <v>1.6663926373645208E-2</v>
       </c>
@@ -4373,7 +4373,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="11">
         <v>1.2766043377454579E-2</v>
       </c>
@@ -4389,7 +4389,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="12">
         <v>6.9981755246819512E-3</v>
       </c>
@@ -4405,7 +4405,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="25">
+      <c r="A46" s="26">
         <v>39</v>
       </c>
       <c r="B46" s="11">
@@ -4423,7 +4423,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="11">
         <v>1.0799955727171583E-2</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="11">
         <v>7.5018690967697038E-3</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="27"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="11">
         <v>5.6937796070318488E-3</v>
       </c>
@@ -4471,7 +4471,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="25">
+      <c r="A50" s="26">
         <v>40</v>
       </c>
       <c r="B50" s="10">
@@ -4489,7 +4489,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="11">
         <v>8.9092473543583659E-3</v>
       </c>
@@ -4505,7 +4505,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="11">
         <v>5.7498961550364394E-3</v>
       </c>
@@ -4521,7 +4521,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="27"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="12">
         <v>4.5518696370374454E-3</v>
       </c>
@@ -4537,7 +4537,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="25">
+      <c r="A54" s="26">
         <v>41</v>
       </c>
       <c r="B54" s="11"/>
@@ -4553,7 +4553,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="11"/>
       <c r="C55" s="5">
         <v>2.0578724119104616E-3</v>
@@ -4567,7 +4567,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="27"/>
       <c r="B56" s="11"/>
       <c r="C56" s="5">
         <v>7.1395573474444579E-4</v>
@@ -4581,7 +4581,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="27"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="11"/>
       <c r="C57" s="5">
         <v>1.6798958464575196E-4</v>
@@ -4595,7 +4595,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="25">
+      <c r="A58" s="26">
         <v>42</v>
       </c>
       <c r="B58" s="10"/>
@@ -4611,7 +4611,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="11"/>
       <c r="C59" s="5">
         <v>1.2599218848431397E-4</v>
@@ -4625,7 +4625,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="11"/>
       <c r="C60" s="5">
         <v>3.3597916929150391E-4</v>
@@ -4639,7 +4639,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="27"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="12"/>
       <c r="C61" s="7">
         <v>1.2599218848431397E-4</v>
@@ -4653,7 +4653,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="26">
+      <c r="A62" s="27">
         <v>43</v>
       </c>
       <c r="B62" s="11"/>
@@ -4669,7 +4669,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="27"/>
       <c r="B63" s="11"/>
       <c r="C63" s="5">
         <v>8.3994792322875979E-5</v>
@@ -4683,7 +4683,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="11"/>
       <c r="C64" s="5">
         <v>0</v>
@@ -4697,7 +4697,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="27"/>
+      <c r="A65" s="28"/>
       <c r="B65" s="11"/>
       <c r="C65" s="5">
         <v>0</v>
@@ -4711,7 +4711,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="25">
+      <c r="A66" s="26">
         <v>44</v>
       </c>
       <c r="B66" s="10"/>
@@ -4727,7 +4727,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="11"/>
       <c r="C67" s="5">
         <v>0</v>
@@ -4741,7 +4741,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
+      <c r="A68" s="27"/>
       <c r="B68" s="11"/>
       <c r="C68" s="5">
         <v>0</v>
@@ -4755,7 +4755,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="27"/>
+      <c r="A69" s="28"/>
       <c r="B69" s="12"/>
       <c r="C69" s="7">
         <v>0</v>
@@ -4769,7 +4769,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="25">
+      <c r="A70" s="26">
         <v>45</v>
       </c>
       <c r="B70" s="11"/>
@@ -4785,7 +4785,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="27"/>
       <c r="B71" s="11"/>
       <c r="C71" s="5">
         <v>0</v>
@@ -4799,7 +4799,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="27"/>
       <c r="B72" s="11"/>
       <c r="C72" s="5">
         <v>0</v>
@@ -4813,7 +4813,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="27"/>
+      <c r="A73" s="28"/>
       <c r="B73" s="11"/>
       <c r="C73" s="5">
         <v>0</v>
@@ -4827,7 +4827,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="25">
+      <c r="A74" s="26">
         <v>46</v>
       </c>
       <c r="B74" s="10"/>
@@ -4843,7 +4843,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="11"/>
       <c r="C75" s="5">
         <v>0</v>
@@ -4857,7 +4857,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
+      <c r="A76" s="27"/>
       <c r="B76" s="11"/>
       <c r="C76" s="5">
         <v>0</v>
@@ -4871,7 +4871,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="27"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="12"/>
       <c r="C77" s="7">
         <v>0</v>
@@ -4886,17 +4886,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
@@ -4905,6 +4894,17 @@
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5198,7 +5198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6174EEDB-7B7A-44D2-9EE9-2214797252C5}">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -5544,7 +5544,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="28">
+      <c r="F21" s="25">
         <f>SUM(F3:F20)</f>
         <v>1.0199999999999998</v>
       </c>
@@ -5578,8 +5578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A7BE78-C8A2-4AA0-A137-4EE20A67C024}">
   <dimension ref="B3:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5749,7 +5749,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="28">
+      <c r="D14" s="25">
         <f>SUM(D4:D13)</f>
         <v>1</v>
       </c>
@@ -5781,12 +5781,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5990,17 +5989,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6024,17 +6032,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
idk why this is here again, xlsx is weird in git
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1758102-C42F-4C1A-9D36-173235FAB1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C636F47-E8D2-43C2-85C3-394B05EDCE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="5715" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="3" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-27990" yWindow="5715" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -5198,7 +5198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6174EEDB-7B7A-44D2-9EE9-2214797252C5}">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -5578,7 +5578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A7BE78-C8A2-4AA0-A137-4EE20A67C024}">
   <dimension ref="B3:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
still messing with the new data
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C636F47-E8D2-43C2-85C3-394B05EDCE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C554F0F9-4127-4390-972C-3F4D74CD970C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="5715" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="2" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="1830" yWindow="765" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="3" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -4886,6 +4886,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
@@ -4894,17 +4905,6 @@
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5198,7 +5198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6174EEDB-7B7A-44D2-9EE9-2214797252C5}">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -5578,8 +5578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A7BE78-C8A2-4AA0-A137-4EE20A67C024}">
   <dimension ref="B3:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5781,11 +5781,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5989,26 +5990,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6032,9 +6024,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
data and management scenario tinkering after call with Craig
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
+++ b/Data/Nisqually/Nisqually_Chinook_and_Chum_from_Craig_July2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C554F0F9-4127-4390-972C-3F4D74CD970C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E192F-4E3E-4436-B2F3-469E6C3915D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="765" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="3" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-28140" yWindow="5865" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="1" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -4886,17 +4886,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
@@ -4905,6 +4894,17 @@
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4915,7 +4915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5AB5EB-5F17-4CB3-ADB0-B51E1B4ACDBA}">
   <dimension ref="D4:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -5578,8 +5578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A7BE78-C8A2-4AA0-A137-4EE20A67C024}">
   <dimension ref="B3:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5781,12 +5781,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5990,17 +5989,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6024,17 +6032,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f5b128de-c6a3-4183-b93b-b89b90348e84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>